<commit_message>
can send helics messages from values that are vectors or on buses
</commit_message>
<xml_diff>
--- a/examples/External_interfacing_example/pyDSS_project/PyDSS Scenarios/helics_interface/ExportLists/ExportMode-byElement.xlsx
+++ b/examples/External_interfacing_example/pyDSS_project/PyDSS Scenarios/helics_interface/ExportLists/ExportMode-byElement.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD3DA08-4154-4CB8-9873-BE8D39B9C047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A2A18C-305A-4136-83E4-D2DC4126BA6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3270" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,16 +535,16 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -554,7 +554,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -568,7 +568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -580,7 +580,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>

</xml_diff>